<commit_message>
project: update 20220908-p8_instr.xlsx and UM_10_16Table.xlsx.
</commit_message>
<xml_diff>
--- a/data/meta/20220908-p8_instr.xlsx
+++ b/data/meta/20220908-p8_instr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27100" windowHeight="15540"/>
+    <workbookView windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="20220908_p8_instr" sheetId="1" r:id="rId1"/>
@@ -3700,7 +3700,7 @@
     <t>addeo</t>
   </si>
   <si>
-    <t>1 - 2 cycles (GPR) ; 2 cycles (XER) ; 5 cycles (CR); if with dot suffix: 1聽- 2 cycles (GPR) ; 2聽- 3 cycles (XER) ; 6 - 7 cycles (CR)</t>
+    <t>1 - 2 cycles (GPR) ; 2 cycles (XER) ; 5 cycles (CR); if with dot suffix: 1 - 2 cycles (GPR) ; 2 - 3 cycles (XER) ; 6 - 7 cycles (CR)</t>
   </si>
   <si>
     <t>Add Extended &amp; record OV XO-form</t>
@@ -6612,10 +6612,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -6655,28 +6655,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -6687,17 +6665,17 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6719,14 +6697,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6742,7 +6713,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6750,7 +6735,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6764,7 +6749,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6785,7 +6785,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6797,25 +6803,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6827,79 +6827,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6917,13 +6851,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6935,7 +6875,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6947,19 +6905,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6992,16 +6992,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7021,43 +7047,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7075,22 +7075,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7102,61 +7102,61 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7168,34 +7168,34 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7204,13 +7204,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7546,16 +7546,10 @@
   <dimension ref="A1:I756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="68.9134615384615" defaultRowHeight="16.8"/>
-  <cols>
-    <col min="1" max="1" width="14.4615384615385" customWidth="1"/>
-    <col min="2" max="2" width="44.5480769230769" customWidth="1"/>
-    <col min="3" max="3" width="44.8653846153846" customWidth="1"/>
-    <col min="4" max="16384" width="68.9134615384615" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">

</xml_diff>